<commit_message>
Fixed ForHome6, changed all tests and finished ForHome7. Started Homework1
</commit_message>
<xml_diff>
--- a/ForHome6/Engineering/model_report_engineering_task03.xlsx
+++ b/ForHome6/Engineering/model_report_engineering_task03.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t xml:space="preserve">Model</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">logistic model on Index(['Male', 'age', 'db', 'alkphos', 'sgot', 'alb', 'has_liver_disease'], dtype='object')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the best model, because it’s the simplest model.</t>
   </si>
   <si>
     <t xml:space="preserve">svm model on Index(['Male', 'age', 'db', 'alkphos', 'sgot', 'alb', 'has_liver_disease'], dtype='object')</t>
@@ -151,12 +154,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFAFD095"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -206,6 +215,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -215,6 +232,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFAFD095"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -228,10 +305,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6100560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:rowOff>4570920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -245,7 +322,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24053760" y="350640"/>
-          <a:ext cx="6100920" cy="4571280"/>
+          <a:ext cx="6100560" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -265,10 +342,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6100560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:rowOff>4570920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -282,7 +359,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24053760" y="4922640"/>
-          <a:ext cx="6100920" cy="4571280"/>
+          <a:ext cx="6100560" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -302,10 +379,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6100560</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:rowOff>4570920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -319,7 +396,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24053760" y="9494640"/>
-          <a:ext cx="6100920" cy="4571280"/>
+          <a:ext cx="6100560" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -339,10 +416,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6100560</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:rowOff>4570920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -356,7 +433,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24053760" y="14066640"/>
-          <a:ext cx="6100920" cy="4571280"/>
+          <a:ext cx="6100560" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -376,10 +453,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6100560</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:rowOff>4570920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -393,7 +470,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24053760" y="18638640"/>
-          <a:ext cx="6100920" cy="4571280"/>
+          <a:ext cx="6100560" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -413,10 +490,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6100560</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:rowOff>4570920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -430,7 +507,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24053760" y="23210640"/>
-          <a:ext cx="6100920" cy="4571280"/>
+          <a:ext cx="6100560" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -450,10 +527,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6100560</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:rowOff>4570920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -467,7 +544,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24053760" y="27782640"/>
-          <a:ext cx="6100920" cy="4571280"/>
+          <a:ext cx="6100560" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -487,10 +564,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6100560</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:rowOff>4570920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -504,7 +581,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24053760" y="32354640"/>
-          <a:ext cx="6100920" cy="4571280"/>
+          <a:ext cx="6100560" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -524,10 +601,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6100560</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:rowOff>4570920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -541,7 +618,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24053760" y="36926640"/>
-          <a:ext cx="6100920" cy="4571280"/>
+          <a:ext cx="6100560" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -557,14 +634,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>26640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>141480</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>4571280</xdr:rowOff>
+      <xdr:colOff>141120</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -577,8 +654,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="18638640"/>
-          <a:ext cx="6095160" cy="4571280"/>
+          <a:off x="0" y="41525280"/>
+          <a:ext cx="6094800" cy="4570920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -601,10 +678,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -623,8 +700,8 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -638,7 +715,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="33.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="35.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="95.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.73"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="12" style="1" width="11.54"/>
   </cols>
@@ -875,44 +952,47 @@
         <v>20.0721153846154</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="360" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="9" s="3" customFormat="true" ht="360" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="n">
+      <c r="D9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3" t="n">
         <v>40.1442307692308</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1" t="n">
+      <c r="F9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="n">
         <v>20.0721153846154</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="360" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>1</v>
@@ -935,13 +1015,13 @@
     </row>
     <row r="11" customFormat="false" ht="360" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="n">
         <v>1</v>

</xml_diff>